<commit_message>
feat: Implement optimized cancer cell prediction model training, evaluation, and comprehensive Excel reporting with charts.
</commit_message>
<xml_diff>
--- a/AI_PES - Inferno OptimizedCode/AI_PES - Inferno FinalPredictionChart.xlsx
+++ b/AI_PES - Inferno OptimizedCode/AI_PES - Inferno FinalPredictionChart.xlsx
@@ -138,7 +138,6 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
   <chart>
     <title>
       <tx>
@@ -149,40 +148,37 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Actual vs Predicted</a:t>
+              <a:t>Key Performance Metrics</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
     </title>
     <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>Actual</v>
+            <strRef>
+              <f>'Final Analysis'!AH1</f>
+            </strRef>
           </tx>
           <spPr>
             <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
+          <cat>
+            <numRef>
+              <f>'Final Analysis'!$AG$2:$AG$5</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Final Analysis'!$Z$1:$Z$205</f>
+              <f>'Final Analysis'!$AH$2:$AH$5</f>
             </numRef>
           </val>
         </ser>
@@ -190,33 +186,175 @@
           <idx val="1"/>
           <order val="1"/>
           <tx>
-            <v>Predicted</v>
+            <strRef>
+              <f>'Final Analysis'!AI1</f>
+            </strRef>
           </tx>
           <spPr>
             <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
+          <cat>
+            <numRef>
+              <f>'Final Analysis'!$AG$2:$AG$5</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Final Analysis'!$AA$1:$AA$205</f>
+              <f>'Final Analysis'!$AI$2:$AI$5</f>
             </numRef>
           </val>
         </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Final Analysis'!AJ1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Final Analysis'!$AG$2:$AG$5</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Final Analysis'!$AJ$2:$AJ$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
-      </lineChart>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Model</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Score</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Top 10 Feature Importance</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="bar"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Final Analysis'!AH9</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Final Analysis'!$AG$10:$AG$19</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Final Analysis'!$AH$10:$AH$19</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <dLblPos val="outEnd"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
       <catAx>
         <axId val="10"/>
         <scaling>
@@ -232,7 +370,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Patient Index</a:t>
+                  <a:t>Feature</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -259,7 +397,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Diagnosis (0=Neg, 1=Pos)</a:t>
+                  <a:t>Importance</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -270,9 +408,122 @@
         <crossAx val="10"/>
       </valAx>
     </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Model Confidence (How sure is it?)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Final Analysis'!AH23</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Final Analysis'!$AG$24:$AG$28</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Final Analysis'!$AH$24:$AH$28</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <dLblPos val="outEnd"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Confidence %</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Count of Patients</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
@@ -283,12 +534,12 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>30</col>
+      <col>39</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <ext cx="9000000" cy="5400000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -298,6 +549,50 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>39</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9000000" cy="5400000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>39</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9000000" cy="5400000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -595,7 +890,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI205"/>
+  <dimension ref="A1:AK205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,27 +1039,37 @@
           <t>Prediction_Probability</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Model_Confidence</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Conf_Bin</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>ROC-AUC</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>F1 Score</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Log Loss</t>
         </is>
@@ -855,22 +1160,30 @@
       <c r="AB2" t="n">
         <v>0.35</v>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AC2" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>Logistic Regression</t>
         </is>
       </c>
-      <c r="AF2" t="n">
-        <v>0.8872549019607843</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.9272939801285798</v>
-      </c>
       <c r="AH2" t="n">
-        <v>0.780952380952381</v>
+        <v>0.89</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.2965370678984829</v>
+        <v>0.93</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="3">
@@ -958,22 +1271,30 @@
       <c r="AB3" t="n">
         <v>0.76</v>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AC3" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>Decision Tree</t>
         </is>
       </c>
-      <c r="AF3" t="n">
-        <v>0.8529411764705882</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.7641145528930451</v>
-      </c>
       <c r="AH3" t="n">
-        <v>0.6938775510204082</v>
+        <v>0.85</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.4284981525592481</v>
+        <v>0.76</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.43</v>
       </c>
     </row>
     <row r="4">
@@ -1061,22 +1382,30 @@
       <c r="AB4" t="n">
         <v>0.035</v>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AC4" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>Random Forest</t>
         </is>
       </c>
-      <c r="AF4" t="n">
-        <v>0.8970588235294118</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0.9364699006428989</v>
-      </c>
       <c r="AH4" t="n">
-        <v>0.7961165048543689</v>
+        <v>0.9</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.326345725748409</v>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.33</v>
       </c>
     </row>
     <row r="5">
@@ -1164,22 +1493,30 @@
       <c r="AB5" t="n">
         <v>0.68</v>
       </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AC5" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
         <is>
           <t>Gradient Boosting</t>
         </is>
       </c>
-      <c r="AF5" t="n">
-        <v>0.8823529411764706</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.907071887784921</v>
-      </c>
       <c r="AH5" t="n">
-        <v>0.7692307692307693</v>
+        <v>0.88</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.3384284416230885</v>
+        <v>0.91</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.34</v>
       </c>
     </row>
     <row r="6">
@@ -1267,6 +1604,14 @@
       <c r="AB6" t="n">
         <v>0.48</v>
       </c>
+      <c r="AC6" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1353,6 +1698,14 @@
       <c r="AB7" t="n">
         <v>0.515</v>
       </c>
+      <c r="AC7" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1439,6 +1792,14 @@
       <c r="AB8" t="n">
         <v>0.375</v>
       </c>
+      <c r="AC8" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1525,6 +1886,24 @@
       <c r="AB9" t="n">
         <v>0.265</v>
       </c>
+      <c r="AC9" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AG9" s="1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="AH9" s="1" t="inlineStr">
+        <is>
+          <t>Importance</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1611,6 +1990,22 @@
       <c r="AB10" t="n">
         <v>0.08</v>
       </c>
+      <c r="AC10" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>Family_Cancer_History_Yes</t>
+        </is>
+      </c>
+      <c r="AH10" t="n">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1697,6 +2092,22 @@
       <c r="AB11" t="n">
         <v>0.315</v>
       </c>
+      <c r="AC11" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>Genetic_Markers_Present</t>
+        </is>
+      </c>
+      <c r="AH11" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1783,6 +2194,22 @@
       <c r="AB12" t="n">
         <v>0.235</v>
       </c>
+      <c r="AC12" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>Tobacco_Usage</t>
+        </is>
+      </c>
+      <c r="AH12" t="n">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1869,6 +2296,22 @@
       <c r="AB13" t="n">
         <v>0.325</v>
       </c>
+      <c r="AC13" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1955,6 +2398,22 @@
       <c r="AB14" t="n">
         <v>0.02</v>
       </c>
+      <c r="AC14" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>Hemoglobin_Level</t>
+        </is>
+      </c>
+      <c r="AH14" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2041,6 +2500,22 @@
       <c r="AB15" t="n">
         <v>0.1</v>
       </c>
+      <c r="AC15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="AH15" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2127,6 +2602,22 @@
       <c r="AB16" t="n">
         <v>0.615</v>
       </c>
+      <c r="AC16" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>Physical_Activity</t>
+        </is>
+      </c>
+      <c r="AH16" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2213,6 +2704,22 @@
       <c r="AB17" t="n">
         <v>0.265</v>
       </c>
+      <c r="AC17" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>WBC_RBC_Ratio</t>
+        </is>
+      </c>
+      <c r="AH17" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2299,6 +2806,22 @@
       <c r="AB18" t="n">
         <v>0.165</v>
       </c>
+      <c r="AC18" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>Platelet_Count</t>
+        </is>
+      </c>
+      <c r="AH18" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2385,6 +2908,22 @@
       <c r="AB19" t="n">
         <v>0.08</v>
       </c>
+      <c r="AC19" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>BP_Product</t>
+        </is>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2471,6 +3010,14 @@
       <c r="AB20" t="n">
         <v>0.39</v>
       </c>
+      <c r="AC20" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2557,6 +3104,14 @@
       <c r="AB21" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC21" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2643,6 +3198,14 @@
       <c r="AB22" t="n">
         <v>0.07000000000000001</v>
       </c>
+      <c r="AC22" t="n">
+        <v>0.9299999999999999</v>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2729,6 +3292,24 @@
       <c r="AB23" t="n">
         <v>0.14</v>
       </c>
+      <c r="AC23" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AG23" s="1" t="inlineStr">
+        <is>
+          <t>Confidence Level</t>
+        </is>
+      </c>
+      <c r="AH23" s="1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2815,6 +3396,22 @@
       <c r="AB24" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC24" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
+      <c r="AH24" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2901,6 +3498,22 @@
       <c r="AB25" t="n">
         <v>0.17</v>
       </c>
+      <c r="AC25" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
+      <c r="AH25" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2987,6 +3600,22 @@
       <c r="AB26" t="n">
         <v>0.05</v>
       </c>
+      <c r="AC26" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AH26" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3073,6 +3702,22 @@
       <c r="AB27" t="n">
         <v>0.9</v>
       </c>
+      <c r="AC27" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="AH27" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -3159,6 +3804,22 @@
       <c r="AB28" t="n">
         <v>0.245</v>
       </c>
+      <c r="AC28" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
+      <c r="AH28" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3245,6 +3906,14 @@
       <c r="AB29" t="n">
         <v>0.245</v>
       </c>
+      <c r="AC29" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -3331,6 +4000,14 @@
       <c r="AB30" t="n">
         <v>0.015</v>
       </c>
+      <c r="AC30" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3417,6 +4094,14 @@
       <c r="AB31" t="n">
         <v>0.175</v>
       </c>
+      <c r="AC31" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3503,6 +4188,14 @@
       <c r="AB32" t="n">
         <v>0.74</v>
       </c>
+      <c r="AC32" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3589,6 +4282,14 @@
       <c r="AB33" t="n">
         <v>0.365</v>
       </c>
+      <c r="AC33" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3675,6 +4376,14 @@
       <c r="AB34" t="n">
         <v>0.39</v>
       </c>
+      <c r="AC34" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -3761,6 +4470,14 @@
       <c r="AB35" t="n">
         <v>0.76</v>
       </c>
+      <c r="AC35" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3847,6 +4564,14 @@
       <c r="AB36" t="n">
         <v>0.235</v>
       </c>
+      <c r="AC36" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="AD36" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3933,6 +4658,14 @@
       <c r="AB37" t="n">
         <v>0.05</v>
       </c>
+      <c r="AC37" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4019,6 +4752,14 @@
       <c r="AB38" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC38" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -4105,6 +4846,14 @@
       <c r="AB39" t="n">
         <v>0.175</v>
       </c>
+      <c r="AC39" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4191,6 +4940,14 @@
       <c r="AB40" t="n">
         <v>0.545</v>
       </c>
+      <c r="AC40" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="AD40" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -4277,6 +5034,14 @@
       <c r="AB41" t="n">
         <v>0.01</v>
       </c>
+      <c r="AC41" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -4363,6 +5128,14 @@
       <c r="AB42" t="n">
         <v>0.44</v>
       </c>
+      <c r="AC42" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -4449,6 +5222,14 @@
       <c r="AB43" t="n">
         <v>0.29</v>
       </c>
+      <c r="AC43" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="AD43" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4535,6 +5316,14 @@
       <c r="AB44" t="n">
         <v>0.5600000000000001</v>
       </c>
+      <c r="AC44" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4621,6 +5410,14 @@
       <c r="AB45" t="n">
         <v>0.025</v>
       </c>
+      <c r="AC45" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4707,6 +5504,14 @@
       <c r="AB46" t="n">
         <v>0.065</v>
       </c>
+      <c r="AC46" t="n">
+        <v>0.9350000000000001</v>
+      </c>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -4793,6 +5598,14 @@
       <c r="AB47" t="n">
         <v>0.01</v>
       </c>
+      <c r="AC47" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -4879,6 +5692,14 @@
       <c r="AB48" t="n">
         <v>0.08500000000000001</v>
       </c>
+      <c r="AC48" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -4965,6 +5786,14 @@
       <c r="AB49" t="n">
         <v>0.23</v>
       </c>
+      <c r="AC49" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -5051,6 +5880,14 @@
       <c r="AB50" t="n">
         <v>0.065</v>
       </c>
+      <c r="AC50" t="n">
+        <v>0.9350000000000001</v>
+      </c>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -5137,6 +5974,14 @@
       <c r="AB51" t="n">
         <v>0.775</v>
       </c>
+      <c r="AC51" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5223,6 +6068,14 @@
       <c r="AB52" t="n">
         <v>0.225</v>
       </c>
+      <c r="AC52" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -5309,6 +6162,14 @@
       <c r="AB53" t="n">
         <v>0.345</v>
       </c>
+      <c r="AC53" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -5395,6 +6256,14 @@
       <c r="AB54" t="n">
         <v>0.605</v>
       </c>
+      <c r="AC54" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -5481,6 +6350,14 @@
       <c r="AB55" t="n">
         <v>0.715</v>
       </c>
+      <c r="AC55" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -5567,6 +6444,14 @@
       <c r="AB56" t="n">
         <v>0.005</v>
       </c>
+      <c r="AC56" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -5653,6 +6538,14 @@
       <c r="AB57" t="n">
         <v>0.095</v>
       </c>
+      <c r="AC57" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -5739,6 +6632,14 @@
       <c r="AB58" t="n">
         <v>0.15</v>
       </c>
+      <c r="AC58" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -5825,6 +6726,14 @@
       <c r="AB59" t="n">
         <v>0.125</v>
       </c>
+      <c r="AC59" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5911,6 +6820,14 @@
       <c r="AB60" t="n">
         <v>0.32</v>
       </c>
+      <c r="AC60" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5997,6 +6914,14 @@
       <c r="AB61" t="n">
         <v>0.205</v>
       </c>
+      <c r="AC61" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6083,6 +7008,14 @@
       <c r="AB62" t="n">
         <v>0.135</v>
       </c>
+      <c r="AC62" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -6169,6 +7102,14 @@
       <c r="AB63" t="n">
         <v>0.02</v>
       </c>
+      <c r="AC63" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AD63" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -6255,6 +7196,14 @@
       <c r="AB64" t="n">
         <v>0.375</v>
       </c>
+      <c r="AC64" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="AD64" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -6341,6 +7290,14 @@
       <c r="AB65" t="n">
         <v>0.575</v>
       </c>
+      <c r="AC65" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="AD65" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6427,6 +7384,14 @@
       <c r="AB66" t="n">
         <v>0.545</v>
       </c>
+      <c r="AC66" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6513,6 +7478,14 @@
       <c r="AB67" t="n">
         <v>0.7</v>
       </c>
+      <c r="AC67" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -6599,6 +7572,14 @@
       <c r="AB68" t="n">
         <v>0.2</v>
       </c>
+      <c r="AC68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AD68" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -6685,6 +7666,14 @@
       <c r="AB69" t="n">
         <v>0.095</v>
       </c>
+      <c r="AC69" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="AD69" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6771,6 +7760,14 @@
       <c r="AB70" t="n">
         <v>0.01</v>
       </c>
+      <c r="AC70" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AD70" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -6857,6 +7854,14 @@
       <c r="AB71" t="n">
         <v>0.58</v>
       </c>
+      <c r="AC71" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="AD71" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -6943,6 +7948,14 @@
       <c r="AB72" t="n">
         <v>0.21</v>
       </c>
+      <c r="AC72" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="AD72" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -7029,6 +8042,14 @@
       <c r="AB73" t="n">
         <v>0.19</v>
       </c>
+      <c r="AC73" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AD73" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -7115,6 +8136,14 @@
       <c r="AB74" t="n">
         <v>0.155</v>
       </c>
+      <c r="AC74" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="AD74" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -7201,6 +8230,14 @@
       <c r="AB75" t="n">
         <v>0.855</v>
       </c>
+      <c r="AC75" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="AD75" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -7287,6 +8324,14 @@
       <c r="AB76" t="n">
         <v>0.57</v>
       </c>
+      <c r="AC76" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="AD76" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -7373,6 +8418,14 @@
       <c r="AB77" t="n">
         <v>0.09</v>
       </c>
+      <c r="AC77" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AD77" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7459,6 +8512,14 @@
       <c r="AB78" t="n">
         <v>0.62</v>
       </c>
+      <c r="AC78" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AD78" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -7545,6 +8606,14 @@
       <c r="AB79" t="n">
         <v>0.145</v>
       </c>
+      <c r="AC79" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="AD79" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -7631,6 +8700,14 @@
       <c r="AB80" t="n">
         <v>0.16</v>
       </c>
+      <c r="AC80" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AD80" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -7717,6 +8794,14 @@
       <c r="AB81" t="n">
         <v>0.755</v>
       </c>
+      <c r="AC81" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="AD81" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -7803,6 +8888,14 @@
       <c r="AB82" t="n">
         <v>0.61</v>
       </c>
+      <c r="AC82" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="AD82" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -7889,6 +8982,14 @@
       <c r="AB83" t="n">
         <v>0.6899999999999999</v>
       </c>
+      <c r="AC83" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="AD83" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -7975,6 +9076,14 @@
       <c r="AB84" t="n">
         <v>0.01</v>
       </c>
+      <c r="AC84" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AD84" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -8061,6 +9170,14 @@
       <c r="AB85" t="n">
         <v>0.215</v>
       </c>
+      <c r="AC85" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="AD85" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -8147,6 +9264,14 @@
       <c r="AB86" t="n">
         <v>0.15</v>
       </c>
+      <c r="AC86" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AD86" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -8233,6 +9358,14 @@
       <c r="AB87" t="n">
         <v>0.59</v>
       </c>
+      <c r="AC87" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="AD87" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -8319,6 +9452,14 @@
       <c r="AB88" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC88" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD88" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -8405,6 +9546,14 @@
       <c r="AB89" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC89" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD89" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -8491,6 +9640,14 @@
       <c r="AB90" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC90" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD90" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -8577,6 +9734,14 @@
       <c r="AB91" t="n">
         <v>0.01</v>
       </c>
+      <c r="AC91" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AD91" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -8663,6 +9828,14 @@
       <c r="AB92" t="n">
         <v>0.1</v>
       </c>
+      <c r="AC92" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AD92" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -8749,6 +9922,14 @@
       <c r="AB93" t="n">
         <v>0.02</v>
       </c>
+      <c r="AC93" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AD93" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -8835,6 +10016,14 @@
       <c r="AB94" t="n">
         <v>0.19</v>
       </c>
+      <c r="AC94" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AD94" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -8921,6 +10110,14 @@
       <c r="AB95" t="n">
         <v>0.37</v>
       </c>
+      <c r="AC95" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="AD95" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -9007,6 +10204,14 @@
       <c r="AB96" t="n">
         <v>0.875</v>
       </c>
+      <c r="AC96" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="AD96" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -9093,6 +10298,14 @@
       <c r="AB97" t="n">
         <v>0.715</v>
       </c>
+      <c r="AC97" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="AD97" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -9179,6 +10392,14 @@
       <c r="AB98" t="n">
         <v>0.28</v>
       </c>
+      <c r="AC98" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AD98" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -9265,6 +10486,14 @@
       <c r="AB99" t="n">
         <v>0.06</v>
       </c>
+      <c r="AC99" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AD99" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -9351,6 +10580,14 @@
       <c r="AB100" t="n">
         <v>0.305</v>
       </c>
+      <c r="AC100" t="n">
+        <v>0.6950000000000001</v>
+      </c>
+      <c r="AD100" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -9437,6 +10674,14 @@
       <c r="AB101" t="n">
         <v>0.185</v>
       </c>
+      <c r="AC101" t="n">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="AD101" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -9523,6 +10768,14 @@
       <c r="AB102" t="n">
         <v>0.15</v>
       </c>
+      <c r="AC102" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AD102" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -9609,6 +10862,14 @@
       <c r="AB103" t="n">
         <v>0.66</v>
       </c>
+      <c r="AC103" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="AD103" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -9695,6 +10956,14 @@
       <c r="AB104" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC104" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD104" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9781,6 +11050,14 @@
       <c r="AB105" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC105" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD105" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9867,6 +11144,14 @@
       <c r="AB106" t="n">
         <v>0.08</v>
       </c>
+      <c r="AC106" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AD106" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9953,6 +11238,14 @@
       <c r="AB107" t="n">
         <v>0.115</v>
       </c>
+      <c r="AC107" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="AD107" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10039,6 +11332,14 @@
       <c r="AB108" t="n">
         <v>0.64</v>
       </c>
+      <c r="AC108" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="AD108" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10125,6 +11426,14 @@
       <c r="AB109" t="n">
         <v>0.14</v>
       </c>
+      <c r="AC109" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AD109" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10211,6 +11520,14 @@
       <c r="AB110" t="n">
         <v>0.425</v>
       </c>
+      <c r="AC110" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="AD110" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10297,6 +11614,14 @@
       <c r="AB111" t="n">
         <v>0.17</v>
       </c>
+      <c r="AC111" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="AD111" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10383,6 +11708,14 @@
       <c r="AB112" t="n">
         <v>0.78</v>
       </c>
+      <c r="AC112" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AD112" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -10469,6 +11802,14 @@
       <c r="AB113" t="n">
         <v>0.03</v>
       </c>
+      <c r="AC113" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="AD113" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10555,6 +11896,14 @@
       <c r="AB114" t="n">
         <v>0.11</v>
       </c>
+      <c r="AC114" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="AD114" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -10641,6 +11990,14 @@
       <c r="AB115" t="n">
         <v>0.32</v>
       </c>
+      <c r="AC115" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AD115" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -10727,6 +12084,14 @@
       <c r="AB116" t="n">
         <v>0.76</v>
       </c>
+      <c r="AC116" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AD116" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -10813,6 +12178,14 @@
       <c r="AB117" t="n">
         <v>0.515</v>
       </c>
+      <c r="AC117" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="AD117" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -10899,6 +12272,14 @@
       <c r="AB118" t="n">
         <v>0.575</v>
       </c>
+      <c r="AC118" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="AD118" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -10985,6 +12366,14 @@
       <c r="AB119" t="n">
         <v>0.755</v>
       </c>
+      <c r="AC119" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="AD119" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -11071,6 +12460,14 @@
       <c r="AB120" t="n">
         <v>0.16</v>
       </c>
+      <c r="AC120" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AD120" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -11157,6 +12554,14 @@
       <c r="AB121" t="n">
         <v>0.105</v>
       </c>
+      <c r="AC121" t="n">
+        <v>0.895</v>
+      </c>
+      <c r="AD121" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -11243,6 +12648,14 @@
       <c r="AB122" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC122" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD122" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -11329,6 +12742,14 @@
       <c r="AB123" t="n">
         <v>0.165</v>
       </c>
+      <c r="AC123" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="AD123" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -11415,6 +12836,14 @@
       <c r="AB124" t="n">
         <v>0.055</v>
       </c>
+      <c r="AC124" t="n">
+        <v>0.945</v>
+      </c>
+      <c r="AD124" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -11501,6 +12930,14 @@
       <c r="AB125" t="n">
         <v>0.14</v>
       </c>
+      <c r="AC125" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AD125" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -11587,6 +13024,14 @@
       <c r="AB126" t="n">
         <v>0.11</v>
       </c>
+      <c r="AC126" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="AD126" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -11673,6 +13118,14 @@
       <c r="AB127" t="n">
         <v>0.05</v>
       </c>
+      <c r="AC127" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AD127" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -11759,6 +13212,14 @@
       <c r="AB128" t="n">
         <v>0.095</v>
       </c>
+      <c r="AC128" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="AD128" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -11845,6 +13306,14 @@
       <c r="AB129" t="n">
         <v>0.655</v>
       </c>
+      <c r="AC129" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="AD129" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -11931,6 +13400,14 @@
       <c r="AB130" t="n">
         <v>0.335</v>
       </c>
+      <c r="AC130" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="AD130" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -12017,6 +13494,14 @@
       <c r="AB131" t="n">
         <v>0.075</v>
       </c>
+      <c r="AC131" t="n">
+        <v>0.925</v>
+      </c>
+      <c r="AD131" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -12103,6 +13588,14 @@
       <c r="AB132" t="n">
         <v>0.205</v>
       </c>
+      <c r="AC132" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="AD132" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -12189,6 +13682,14 @@
       <c r="AB133" t="n">
         <v>0.165</v>
       </c>
+      <c r="AC133" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="AD133" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -12275,6 +13776,14 @@
       <c r="AB134" t="n">
         <v>0.095</v>
       </c>
+      <c r="AC134" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="AD134" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -12361,6 +13870,14 @@
       <c r="AB135" t="n">
         <v>0.13</v>
       </c>
+      <c r="AC135" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="AD135" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -12447,6 +13964,14 @@
       <c r="AB136" t="n">
         <v>0.24</v>
       </c>
+      <c r="AC136" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AD136" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -12533,6 +14058,14 @@
       <c r="AB137" t="n">
         <v>0.24</v>
       </c>
+      <c r="AC137" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AD137" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -12619,6 +14152,14 @@
       <c r="AB138" t="n">
         <v>0.03</v>
       </c>
+      <c r="AC138" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="AD138" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -12705,6 +14246,14 @@
       <c r="AB139" t="n">
         <v>0.05</v>
       </c>
+      <c r="AC139" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AD139" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -12791,6 +14340,14 @@
       <c r="AB140" t="n">
         <v>0.205</v>
       </c>
+      <c r="AC140" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="AD140" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -12877,6 +14434,14 @@
       <c r="AB141" t="n">
         <v>0.515</v>
       </c>
+      <c r="AC141" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="AD141" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -12963,6 +14528,14 @@
       <c r="AB142" t="n">
         <v>0.08500000000000001</v>
       </c>
+      <c r="AC142" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="AD142" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -13049,6 +14622,14 @@
       <c r="AB143" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC143" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD143" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -13135,6 +14716,14 @@
       <c r="AB144" t="n">
         <v>0.21</v>
       </c>
+      <c r="AC144" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="AD144" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -13221,6 +14810,14 @@
       <c r="AB145" t="n">
         <v>0.095</v>
       </c>
+      <c r="AC145" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="AD145" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -13307,6 +14904,14 @@
       <c r="AB146" t="n">
         <v>0.135</v>
       </c>
+      <c r="AC146" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="AD146" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -13393,6 +14998,14 @@
       <c r="AB147" t="n">
         <v>0.48</v>
       </c>
+      <c r="AC147" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AD147" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -13479,6 +15092,14 @@
       <c r="AB148" t="n">
         <v>0.08500000000000001</v>
       </c>
+      <c r="AC148" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="AD148" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -13565,6 +15186,14 @@
       <c r="AB149" t="n">
         <v>0.12</v>
       </c>
+      <c r="AC149" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AD149" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -13651,6 +15280,14 @@
       <c r="AB150" t="n">
         <v>0.42</v>
       </c>
+      <c r="AC150" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="AD150" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -13737,6 +15374,14 @@
       <c r="AB151" t="n">
         <v>0.025</v>
       </c>
+      <c r="AC151" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="AD151" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -13823,6 +15468,14 @@
       <c r="AB152" t="n">
         <v>0.015</v>
       </c>
+      <c r="AC152" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="AD152" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -13909,6 +15562,14 @@
       <c r="AB153" t="n">
         <v>0.02</v>
       </c>
+      <c r="AC153" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AD153" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -13995,6 +15656,14 @@
       <c r="AB154" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC154" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD154" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -14081,6 +15750,14 @@
       <c r="AB155" t="n">
         <v>0.32</v>
       </c>
+      <c r="AC155" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AD155" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -14167,6 +15844,14 @@
       <c r="AB156" t="n">
         <v>0.41</v>
       </c>
+      <c r="AC156" t="n">
+        <v>0.5900000000000001</v>
+      </c>
+      <c r="AD156" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -14253,6 +15938,14 @@
       <c r="AB157" t="n">
         <v>0.32</v>
       </c>
+      <c r="AC157" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AD157" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -14339,6 +16032,14 @@
       <c r="AB158" t="n">
         <v>0.12</v>
       </c>
+      <c r="AC158" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AD158" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -14425,6 +16126,14 @@
       <c r="AB159" t="n">
         <v>0.02</v>
       </c>
+      <c r="AC159" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AD159" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -14511,6 +16220,14 @@
       <c r="AB160" t="n">
         <v>0.765</v>
       </c>
+      <c r="AC160" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="AD160" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -14597,6 +16314,14 @@
       <c r="AB161" t="n">
         <v>0.075</v>
       </c>
+      <c r="AC161" t="n">
+        <v>0.925</v>
+      </c>
+      <c r="AD161" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -14683,6 +16408,14 @@
       <c r="AB162" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC162" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD162" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -14769,6 +16502,14 @@
       <c r="AB163" t="n">
         <v>0.155</v>
       </c>
+      <c r="AC163" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="AD163" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -14855,6 +16596,14 @@
       <c r="AB164" t="n">
         <v>0.465</v>
       </c>
+      <c r="AC164" t="n">
+        <v>0.5349999999999999</v>
+      </c>
+      <c r="AD164" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -14941,6 +16690,14 @@
       <c r="AB165" t="n">
         <v>0.175</v>
       </c>
+      <c r="AC165" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="AD165" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -15027,6 +16784,14 @@
       <c r="AB166" t="n">
         <v>0.6</v>
       </c>
+      <c r="AC166" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AD166" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -15113,6 +16878,14 @@
       <c r="AB167" t="n">
         <v>0.155</v>
       </c>
+      <c r="AC167" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="AD167" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -15199,6 +16972,14 @@
       <c r="AB168" t="n">
         <v>0.49</v>
       </c>
+      <c r="AC168" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="AD168" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -15285,6 +17066,14 @@
       <c r="AB169" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC169" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD169" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -15371,6 +17160,14 @@
       <c r="AB170" t="n">
         <v>0.515</v>
       </c>
+      <c r="AC170" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="AD170" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -15457,6 +17254,14 @@
       <c r="AB171" t="n">
         <v>0.15</v>
       </c>
+      <c r="AC171" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AD171" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -15543,6 +17348,14 @@
       <c r="AB172" t="n">
         <v>0.285</v>
       </c>
+      <c r="AC172" t="n">
+        <v>0.7150000000000001</v>
+      </c>
+      <c r="AD172" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -15629,6 +17442,14 @@
       <c r="AB173" t="n">
         <v>0.2</v>
       </c>
+      <c r="AC173" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AD173" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -15715,6 +17536,14 @@
       <c r="AB174" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC174" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD174" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -15801,6 +17630,14 @@
       <c r="AB175" t="n">
         <v>0.055</v>
       </c>
+      <c r="AC175" t="n">
+        <v>0.945</v>
+      </c>
+      <c r="AD175" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -15887,6 +17724,14 @@
       <c r="AB176" t="n">
         <v>0.115</v>
       </c>
+      <c r="AC176" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="AD176" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -15973,6 +17818,14 @@
       <c r="AB177" t="n">
         <v>0.715</v>
       </c>
+      <c r="AC177" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="AD177" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -16059,6 +17912,14 @@
       <c r="AB178" t="n">
         <v>0.04</v>
       </c>
+      <c r="AC178" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="AD178" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -16145,6 +18006,14 @@
       <c r="AB179" t="n">
         <v>0.09</v>
       </c>
+      <c r="AC179" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AD179" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -16231,6 +18100,14 @@
       <c r="AB180" t="n">
         <v>0.08500000000000001</v>
       </c>
+      <c r="AC180" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="AD180" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -16317,6 +18194,14 @@
       <c r="AB181" t="n">
         <v>0.08</v>
       </c>
+      <c r="AC181" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AD181" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -16403,6 +18288,14 @@
       <c r="AB182" t="n">
         <v>0.125</v>
       </c>
+      <c r="AC182" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="AD182" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -16489,6 +18382,14 @@
       <c r="AB183" t="n">
         <v>0.205</v>
       </c>
+      <c r="AC183" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="AD183" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -16575,6 +18476,14 @@
       <c r="AB184" t="n">
         <v>0.045</v>
       </c>
+      <c r="AC184" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="AD184" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -16661,6 +18570,14 @@
       <c r="AB185" t="n">
         <v>0.22</v>
       </c>
+      <c r="AC185" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AD185" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -16747,6 +18664,14 @@
       <c r="AB186" t="n">
         <v>0.15</v>
       </c>
+      <c r="AC186" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AD186" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -16833,6 +18758,14 @@
       <c r="AB187" t="n">
         <v>0.225</v>
       </c>
+      <c r="AC187" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="AD187" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -16919,6 +18852,14 @@
       <c r="AB188" t="n">
         <v>0.08500000000000001</v>
       </c>
+      <c r="AC188" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="AD188" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -17005,6 +18946,14 @@
       <c r="AB189" t="n">
         <v>0.075</v>
       </c>
+      <c r="AC189" t="n">
+        <v>0.925</v>
+      </c>
+      <c r="AD189" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -17091,6 +19040,14 @@
       <c r="AB190" t="n">
         <v>0.4</v>
       </c>
+      <c r="AC190" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AD190" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -17177,6 +19134,14 @@
       <c r="AB191" t="n">
         <v>0.8100000000000001</v>
       </c>
+      <c r="AC191" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AD191" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -17263,6 +19228,14 @@
       <c r="AB192" t="n">
         <v>0.175</v>
       </c>
+      <c r="AC192" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="AD192" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -17349,6 +19322,14 @@
       <c r="AB193" t="n">
         <v>0.735</v>
       </c>
+      <c r="AC193" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="AD193" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -17435,6 +19416,14 @@
       <c r="AB194" t="n">
         <v>0.215</v>
       </c>
+      <c r="AC194" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="AD194" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -17521,6 +19510,14 @@
       <c r="AB195" t="n">
         <v>0.3</v>
       </c>
+      <c r="AC195" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AD195" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -17607,6 +19604,14 @@
       <c r="AB196" t="n">
         <v>0.65</v>
       </c>
+      <c r="AC196" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="AD196" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -17693,6 +19698,14 @@
       <c r="AB197" t="n">
         <v>0.305</v>
       </c>
+      <c r="AC197" t="n">
+        <v>0.6950000000000001</v>
+      </c>
+      <c r="AD197" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -17779,6 +19792,14 @@
       <c r="AB198" t="n">
         <v>0.005</v>
       </c>
+      <c r="AC198" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="AD198" t="inlineStr">
+        <is>
+          <t>90-100%</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -17865,6 +19886,14 @@
       <c r="AB199" t="n">
         <v>0.315</v>
       </c>
+      <c r="AC199" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="AD199" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -17951,6 +19980,14 @@
       <c r="AB200" t="n">
         <v>0.41</v>
       </c>
+      <c r="AC200" t="n">
+        <v>0.5900000000000001</v>
+      </c>
+      <c r="AD200" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -18037,6 +20074,14 @@
       <c r="AB201" t="n">
         <v>0.19</v>
       </c>
+      <c r="AC201" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AD201" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -18123,6 +20168,14 @@
       <c r="AB202" t="n">
         <v>0.57</v>
       </c>
+      <c r="AC202" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="AD202" t="inlineStr">
+        <is>
+          <t>50-60%</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -18209,6 +20262,14 @@
       <c r="AB203" t="n">
         <v>0.6850000000000001</v>
       </c>
+      <c r="AC203" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="AD203" t="inlineStr">
+        <is>
+          <t>60-70%</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -18295,6 +20356,14 @@
       <c r="AB204" t="n">
         <v>0.13</v>
       </c>
+      <c r="AC204" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="AD204" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -18380,6 +20449,14 @@
       </c>
       <c r="AB205" t="n">
         <v>0.72</v>
+      </c>
+      <c r="AC205" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AD205" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>